<commit_message>
Data updated Minor bugs fixed
</commit_message>
<xml_diff>
--- a/vacancies.xlsx
+++ b/vacancies.xlsx
@@ -2202,7 +2202,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -2656,6 +2656,42 @@
         <v>-2</v>
       </c>
       <c r="J12" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-03-22 17:00:10.000000</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>34905</v>
+      </c>
+      <c r="C13" t="n">
+        <v>61</v>
+      </c>
+      <c r="D13" t="n">
+        <v>382</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1700</v>
+      </c>
+      <c r="G13" t="n">
+        <v>9</v>
+      </c>
+      <c r="H13" t="n">
+        <v>3</v>
+      </c>
+      <c r="I13" t="n">
+        <v>-4</v>
+      </c>
+      <c r="J13" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -2787,7 +2823,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -3550,6 +3586,34 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-03-22 17:00:10.000000</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>34905</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>statistic</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Статистика на Djinni за запитом **Харьков**:
+Вакансій за 30 днів: 61
+Кандидати онлайн: 382
+Вилка по зарплаті: $1000-1700
+Відгуків на одну вакансію: 9.0
+https://djinni.co/jobs/tg_search?keywords=%D0%A5%D0%B0%D1%80%D1%8C%D0%BA%D0%BE%D0%B2
+Активність за тиждень:
+Вакансій: +3
+Кандидатів: -4</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>